<commit_message>
Matching function for finance
</commit_message>
<xml_diff>
--- a/app/Views/reportTemplates/Financial_Report_Template - MASTER.xlsx
+++ b/app/Views/reportTemplates/Financial_Report_Template - MASTER.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PAID ENTRIES" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -410,19 +410,7 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -432,6 +420,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -489,7 +489,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -497,7 +497,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.249977111117893"/>
         </left>
@@ -528,7 +528,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -567,7 +567,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -606,7 +606,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -645,7 +645,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -684,7 +684,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -692,7 +692,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.249977111117893"/>
         </left>
@@ -723,7 +723,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -731,7 +731,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.249977111117893"/>
         </left>
@@ -762,7 +762,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -770,7 +770,241 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$UGX]\ * #,##0.00_);_([$UGX]\ * \(#,##0.00\);_([$UGX]\ * &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.249977111117893"/>
         </left>
@@ -1276,123 +1510,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -1838,123 +1955,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.249977111117893"/>
         </left>
@@ -2444,58 +2444,58 @@
     <tableColumn id="3" name="PROFORMA NO." dataDxfId="46"/>
     <tableColumn id="4" name="TAX INVOICE NO." dataDxfId="45"/>
     <tableColumn id="13" name="LPO NO." dataDxfId="44"/>
-    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="43"/>
-    <tableColumn id="6" name="VAT" dataDxfId="42"/>
-    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="41" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="CLEARED" dataDxfId="40"/>
-    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="39"/>
-    <tableColumn id="10" name="CAR REG NO" dataDxfId="38"/>
-    <tableColumn id="11" name="PHONE" dataDxfId="37"/>
-    <tableColumn id="12" name="DATE" dataDxfId="36"/>
+    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="8"/>
+    <tableColumn id="6" name="VAT" dataDxfId="7"/>
+    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="CLEARED" dataDxfId="43"/>
+    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="42"/>
+    <tableColumn id="10" name="CAR REG NO" dataDxfId="41"/>
+    <tableColumn id="11" name="PHONE" dataDxfId="40"/>
+    <tableColumn id="12" name="DATE" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="B7:N28" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="B7:N28" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="B7:N28"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="SN #" dataDxfId="30"/>
-    <tableColumn id="2" name="CUSTOMER NAME" dataDxfId="29"/>
-    <tableColumn id="3" name="PROFORMA NO." dataDxfId="28"/>
-    <tableColumn id="4" name="TAX INVOICE NO." dataDxfId="27"/>
-    <tableColumn id="13" name="LPO NO." dataDxfId="26"/>
-    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="25"/>
-    <tableColumn id="6" name="VAT" dataDxfId="24"/>
-    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="23" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="UNCLEARED" dataDxfId="22"/>
-    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="21"/>
-    <tableColumn id="10" name="CAR REG NO" dataDxfId="20"/>
-    <tableColumn id="11" name="PHONE" dataDxfId="19"/>
-    <tableColumn id="12" name="DATE" dataDxfId="18"/>
+    <tableColumn id="1" name="SN #" dataDxfId="33"/>
+    <tableColumn id="2" name="CUSTOMER NAME" dataDxfId="32"/>
+    <tableColumn id="3" name="PROFORMA NO." dataDxfId="31"/>
+    <tableColumn id="4" name="TAX INVOICE NO." dataDxfId="30"/>
+    <tableColumn id="13" name="LPO NO." dataDxfId="29"/>
+    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="5"/>
+    <tableColumn id="6" name="VAT" dataDxfId="4"/>
+    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="UNCLEARED" dataDxfId="28"/>
+    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="27"/>
+    <tableColumn id="10" name="CAR REG NO" dataDxfId="26"/>
+    <tableColumn id="11" name="PHONE" dataDxfId="25"/>
+    <tableColumn id="12" name="DATE" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B7:N28" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B7:N28" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="B7:N28"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="SN #" dataDxfId="12"/>
-    <tableColumn id="2" name="CUSTOMER NAME" dataDxfId="11"/>
-    <tableColumn id="3" name="PROFORMA NO." dataDxfId="10"/>
-    <tableColumn id="4" name="TAX INVOICE NO." dataDxfId="9"/>
-    <tableColumn id="13" name="LPO NO." dataDxfId="8"/>
-    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="7"/>
-    <tableColumn id="6" name="VAT" dataDxfId="6"/>
-    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="UNCLEARED" dataDxfId="4"/>
-    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="3"/>
-    <tableColumn id="10" name="CAR REG NO" dataDxfId="2"/>
-    <tableColumn id="11" name="PHONE" dataDxfId="1"/>
-    <tableColumn id="12" name="DATE" dataDxfId="0"/>
+    <tableColumn id="1" name="SN #" dataDxfId="18"/>
+    <tableColumn id="2" name="CUSTOMER NAME" dataDxfId="17"/>
+    <tableColumn id="3" name="PROFORMA NO." dataDxfId="16"/>
+    <tableColumn id="4" name="TAX INVOICE NO." dataDxfId="15"/>
+    <tableColumn id="13" name="LPO NO." dataDxfId="14"/>
+    <tableColumn id="5" name="WITHHOLDING TAX" dataDxfId="2"/>
+    <tableColumn id="6" name="VAT" dataDxfId="1"/>
+    <tableColumn id="7" name="TOTAL PAYABLE" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="UNCLEARED" dataDxfId="13"/>
+    <tableColumn id="9" name="CONTACT PERSON" dataDxfId="12"/>
+    <tableColumn id="10" name="CAR REG NO" dataDxfId="11"/>
+    <tableColumn id="11" name="PHONE" dataDxfId="10"/>
+    <tableColumn id="12" name="DATE" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2830,8 +2830,8 @@
   </sheetPr>
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I8" activeCellId="2" sqref="G8:G28 H8:H28 I8:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2969,318 +2969,318 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="21"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="24"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="24"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="16"/>
     </row>
     <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="24"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="16"/>
     </row>
     <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="24"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="21"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="24"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="16"/>
     </row>
     <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="24"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="16"/>
     </row>
     <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="24"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="16"/>
     </row>
     <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="16"/>
     </row>
     <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="20"/>
       <c r="N16" s="16"/>
     </row>
     <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="21"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="24"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="16"/>
     </row>
     <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="24"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="16"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="24"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="16"/>
     </row>
     <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="24"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="16"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="16"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="21"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="16"/>
     </row>
     <row r="23" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="16"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="20"/>
       <c r="N24" s="16"/>
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="20"/>
       <c r="N25" s="16"/>
     </row>
     <row r="26" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="20"/>
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="20"/>
       <c r="N27" s="16"/>
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="25"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="17"/>
     </row>
   </sheetData>
@@ -3314,7 +3314,7 @@
   <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I8" activeCellId="2" sqref="G8:G28 H8:H28 I8:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,318 +3452,318 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="21"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="24"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="24"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="16"/>
     </row>
     <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="24"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="16"/>
     </row>
     <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="24"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="21"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="24"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="16"/>
     </row>
     <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="24"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="16"/>
     </row>
     <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="24"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="16"/>
     </row>
     <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="16"/>
     </row>
     <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="20"/>
       <c r="N16" s="16"/>
     </row>
     <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="21"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="24"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="16"/>
     </row>
     <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="24"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="16"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="24"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="16"/>
     </row>
     <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="24"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="16"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="16"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="21"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="16"/>
     </row>
     <row r="23" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="16"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="20"/>
       <c r="N24" s="16"/>
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="20"/>
       <c r="N25" s="16"/>
     </row>
     <row r="26" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="20"/>
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="20"/>
       <c r="N27" s="16"/>
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="25"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="17"/>
     </row>
   </sheetData>
@@ -3796,8 +3796,8 @@
   </sheetPr>
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:I6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I8" activeCellId="2" sqref="G8:G28 H8:H28 I8:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3935,318 +3935,318 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="21"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="24"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="15"/>
     </row>
     <row r="9" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="24"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="16"/>
     </row>
     <row r="10" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="24"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="16"/>
     </row>
     <row r="11" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="24"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="16"/>
     </row>
     <row r="12" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="21"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="24"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="16"/>
     </row>
     <row r="13" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="24"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="16"/>
     </row>
     <row r="14" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="24"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="16"/>
     </row>
     <row r="15" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="24"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="16"/>
     </row>
     <row r="16" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="24"/>
+      <c r="M16" s="20"/>
       <c r="N16" s="16"/>
     </row>
     <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="21"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="24"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="16"/>
     </row>
     <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="21"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="24"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="16"/>
     </row>
     <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="24"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="16"/>
     </row>
     <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="6"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="24"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="16"/>
     </row>
     <row r="21" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="16"/>
     </row>
     <row r="22" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="21"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="16"/>
     </row>
     <row r="23" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="16"/>
     </row>
     <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="13"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="20"/>
       <c r="N24" s="16"/>
     </row>
     <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="20"/>
       <c r="N25" s="16"/>
     </row>
     <row r="26" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="20"/>
       <c r="N26" s="16"/>
     </row>
     <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="20"/>
       <c r="N27" s="16"/>
     </row>
     <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="14"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="25"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="17"/>
     </row>
   </sheetData>

</xml_diff>